<commit_message>
Add: Ipr Schedules for 4th ORK.
</commit_message>
<xml_diff>
--- a/storage/app/arrivals.xlsx
+++ b/storage/app/arrivals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Smoku\Pfron\pfron-backend\storage\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20284BD-B665-4BC4-BAA1-2571822C9120}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C11238-2FBD-4640-A514-5B3FE6496406}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="644">
   <si>
     <t>Janus</t>
   </si>
@@ -1666,18 +1666,6 @@
     <t>Chamera</t>
   </si>
   <si>
-    <t>23/09/2020</t>
-  </si>
-  <si>
-    <t>23/02/2021</t>
-  </si>
-  <si>
-    <t>24/02/2021</t>
-  </si>
-  <si>
-    <t>25/02/2021</t>
-  </si>
-  <si>
     <t>Andrzejczak</t>
   </si>
   <si>
@@ -1768,131 +1756,236 @@
     <t>Łochowicz</t>
   </si>
   <si>
-    <t>13/09/2019</t>
-  </si>
-  <si>
-    <t>16/09/2019</t>
-  </si>
-  <si>
-    <t>17/09/2019</t>
-  </si>
-  <si>
-    <t>14/10/2019</t>
-  </si>
-  <si>
-    <t>15/10/2019</t>
-  </si>
-  <si>
-    <t>16/10/2019</t>
-  </si>
-  <si>
-    <t>29/01/2020</t>
-  </si>
-  <si>
-    <t>30/01/2020</t>
-  </si>
-  <si>
-    <t>18/09/2019</t>
-  </si>
-  <si>
-    <t>19/09/2019</t>
-  </si>
-  <si>
-    <t>20/09/2019</t>
-  </si>
-  <si>
-    <t>23/09/2019</t>
-  </si>
-  <si>
-    <t>24/09/2019</t>
-  </si>
-  <si>
-    <t>30/09/2019</t>
-  </si>
-  <si>
-    <t>21/10/2019</t>
-  </si>
-  <si>
-    <t>22/10/2019</t>
-  </si>
-  <si>
-    <t>28/01/2020</t>
-  </si>
-  <si>
-    <t>19/10/2020</t>
-  </si>
-  <si>
-    <t>20/10/2020</t>
-  </si>
-  <si>
-    <t>18/01/2021</t>
-  </si>
-  <si>
-    <t>19/01/2021</t>
-  </si>
-  <si>
-    <t>20/01/2021</t>
-  </si>
-  <si>
-    <t>15/03/2021</t>
-  </si>
-  <si>
-    <t>16/03/2021</t>
-  </si>
-  <si>
-    <t>15/09/2019</t>
-  </si>
-  <si>
-    <t>27/01/20</t>
-  </si>
-  <si>
-    <t>26/02/20</t>
-  </si>
-  <si>
-    <t>27/02/20</t>
-  </si>
-  <si>
-    <t>22/09/20</t>
-  </si>
-  <si>
-    <t>26/10/2020</t>
-  </si>
-  <si>
-    <t>27/10/2020</t>
-  </si>
-  <si>
-    <t>13/01/2021</t>
-  </si>
-  <si>
-    <t>22/02/2021</t>
-  </si>
-  <si>
-    <t>25/09/2019</t>
-  </si>
-  <si>
-    <t>26/09/2019</t>
-  </si>
-  <si>
-    <t>24/02/2020</t>
-  </si>
-  <si>
-    <t>25/01/2021</t>
-  </si>
-  <si>
-    <t>26/01/2021</t>
-  </si>
-  <si>
-    <t>17/03/2021</t>
+    <t>2.9.2019</t>
+  </si>
+  <si>
+    <t>3.9.2019</t>
+  </si>
+  <si>
+    <t>4.9.2019</t>
+  </si>
+  <si>
+    <t>5.9.2019</t>
+  </si>
+  <si>
+    <t>9.9.2019</t>
+  </si>
+  <si>
+    <t>10.9.2019</t>
+  </si>
+  <si>
+    <t>11.9.2019</t>
+  </si>
+  <si>
+    <t>12.9.2019</t>
+  </si>
+  <si>
+    <t>9.12.2019</t>
+  </si>
+  <si>
+    <t>10.12.2019</t>
+  </si>
+  <si>
+    <t>11.12.2019</t>
+  </si>
+  <si>
+    <t>11.3.2020</t>
+  </si>
+  <si>
+    <t>1.10.2019</t>
+  </si>
+  <si>
+    <t>4.11.2019</t>
+  </si>
+  <si>
+    <t>5.11.2019</t>
+  </si>
+  <si>
+    <t>9.3.2020</t>
+  </si>
+  <si>
+    <t>10.3.2020</t>
+  </si>
+  <si>
+    <t>8.9.2019</t>
+  </si>
+  <si>
+    <t>8.10.2019</t>
+  </si>
+  <si>
+    <t>9.10.2019</t>
+  </si>
+  <si>
+    <t>10.10.2019</t>
+  </si>
+  <si>
+    <t>9.8.2020</t>
+  </si>
+  <si>
+    <t>10.8.2020</t>
+  </si>
+  <si>
+    <t>12.1.2021</t>
+  </si>
+  <si>
+    <t>8.3.2021</t>
+  </si>
+  <si>
+    <t>9.3.2021</t>
+  </si>
+  <si>
+    <t>2.10.2019</t>
+  </si>
+  <si>
+    <t>3.10.2019</t>
+  </si>
+  <si>
+    <t>6.11.2019</t>
+  </si>
+  <si>
+    <t>7.11.2019</t>
+  </si>
+  <si>
+    <t>7.9.2020</t>
+  </si>
+  <si>
+    <t>13.9.2019</t>
+  </si>
+  <si>
+    <t>16.9.2019</t>
+  </si>
+  <si>
+    <t>17.9.2019</t>
+  </si>
+  <si>
+    <t>14.10.2019</t>
+  </si>
+  <si>
+    <t>15.10.2019</t>
+  </si>
+  <si>
+    <t>16.10.2019</t>
+  </si>
+  <si>
+    <t>29.1.2020</t>
+  </si>
+  <si>
+    <t>30.1.2020</t>
+  </si>
+  <si>
+    <t>23.9.2020</t>
+  </si>
+  <si>
+    <t>23.2.2021</t>
+  </si>
+  <si>
+    <t>24.2.2021</t>
+  </si>
+  <si>
+    <t>25.2.2021</t>
+  </si>
+  <si>
+    <t>18.9.2019</t>
+  </si>
+  <si>
+    <t>19.9.2019</t>
+  </si>
+  <si>
+    <t>20.9.2019</t>
+  </si>
+  <si>
+    <t>23.9.2019</t>
+  </si>
+  <si>
+    <t>24.9.2019</t>
+  </si>
+  <si>
+    <t>30.9.2019</t>
+  </si>
+  <si>
+    <t>21.10.2019</t>
+  </si>
+  <si>
+    <t>22.10.2019</t>
+  </si>
+  <si>
+    <t>28.1.2020</t>
+  </si>
+  <si>
+    <t>19.10.2020</t>
+  </si>
+  <si>
+    <t>20.10.2020</t>
+  </si>
+  <si>
+    <t>18.1.2021</t>
+  </si>
+  <si>
+    <t>19.1.2021</t>
+  </si>
+  <si>
+    <t>20.1.2021</t>
+  </si>
+  <si>
+    <t>15.3.2021</t>
+  </si>
+  <si>
+    <t>16.3.2021</t>
+  </si>
+  <si>
+    <t>15.9.2019</t>
+  </si>
+  <si>
+    <t>27.1.20</t>
+  </si>
+  <si>
+    <t>26.2.20</t>
+  </si>
+  <si>
+    <t>27.2.20</t>
+  </si>
+  <si>
+    <t>22.9.20</t>
+  </si>
+  <si>
+    <t>26.10.2020</t>
+  </si>
+  <si>
+    <t>27.10.2020</t>
+  </si>
+  <si>
+    <t>13.1.2021</t>
+  </si>
+  <si>
+    <t>22.2.2021</t>
+  </si>
+  <si>
+    <t>25.9.2019</t>
+  </si>
+  <si>
+    <t>26.9.2019</t>
+  </si>
+  <si>
+    <t>24.2.2020</t>
+  </si>
+  <si>
+    <t>25.1.2021</t>
+  </si>
+  <si>
+    <t>26.1.2021</t>
+  </si>
+  <si>
+    <t>17.3.2021</t>
+  </si>
+  <si>
+    <t>MARTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1925,6 +2018,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1934,7 +2041,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1983,28 +2090,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2015,41 +2108,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2269,20 +2356,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D239"/>
+  <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="C202" sqref="C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="14"/>
-    <col min="2" max="16384" width="14.42578125" style="7"/>
+    <col min="1" max="1" width="14.42578125" style="11"/>
+    <col min="2" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>425</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2295,9 +2382,9 @@
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>43505</v>
+    <row r="2" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>569</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -2309,9 +2396,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>43505</v>
+    <row r="3" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>569</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -2322,10 +2409,11 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>43533</v>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>570</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -2337,9 +2425,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>43533</v>
+    <row r="5" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>570</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -2351,9 +2439,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>43564</v>
+    <row r="6" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>571</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -2365,12 +2453,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>43564</v>
+    <row r="7" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>571</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -2379,12 +2467,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>43594</v>
+    <row r="8" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>572</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -2393,9 +2481,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>43594</v>
+    <row r="9" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>572</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -2407,9 +2495,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>43717</v>
+    <row r="10" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -2421,9 +2509,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>43717</v>
+    <row r="11" spans="1:7" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -2435,9 +2523,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>43717</v>
+    <row r="12" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>28</v>
@@ -2449,9 +2537,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>43717</v>
+    <row r="13" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>30</v>
@@ -2463,9 +2551,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>43717</v>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
@@ -2477,9 +2565,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>43717</v>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>36</v>
@@ -2491,9 +2579,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>43747</v>
+    <row r="16" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>574</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>39</v>
@@ -2506,8 +2594,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>43747</v>
+      <c r="A17" s="7" t="s">
+        <v>574</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -2520,8 +2608,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>43747</v>
+      <c r="A18" s="7" t="s">
+        <v>574</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>45</v>
@@ -2534,8 +2622,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>43778</v>
+      <c r="A19" s="7" t="s">
+        <v>575</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>48</v>
@@ -2548,8 +2636,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>43778</v>
+      <c r="A20" s="7" t="s">
+        <v>575</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>51</v>
@@ -2562,8 +2650,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>43778</v>
+      <c r="A21" s="7" t="s">
+        <v>575</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>54</v>
@@ -2576,11 +2664,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>43808</v>
+      <c r="A22" s="7" t="s">
+        <v>576</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>57</v>
@@ -2590,8 +2678,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>43808</v>
+      <c r="A23" s="7" t="s">
+        <v>576</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>326</v>
@@ -2604,11 +2692,11 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>43808</v>
+      <c r="A24" s="7" t="s">
+        <v>576</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>60</v>
@@ -2618,11 +2706,11 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>573</v>
+      <c r="A25" s="7" t="s">
+        <v>600</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>62</v>
@@ -2632,8 +2720,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>573</v>
+      <c r="A26" s="7" t="s">
+        <v>600</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>64</v>
@@ -2646,11 +2734,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>574</v>
+      <c r="A27" s="7" t="s">
+        <v>601</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>67</v>
@@ -2660,11 +2748,11 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>574</v>
+      <c r="A28" s="7" t="s">
+        <v>601</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>69</v>
@@ -2674,11 +2762,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>574</v>
+      <c r="A29" s="7" t="s">
+        <v>601</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>71</v>
@@ -2688,11 +2776,11 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>575</v>
+      <c r="A30" s="7" t="s">
+        <v>602</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>73</v>
@@ -2702,11 +2790,11 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>575</v>
+      <c r="A31" s="7" t="s">
+        <v>602</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>75</v>
@@ -2716,8 +2804,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>576</v>
+      <c r="A32" s="7" t="s">
+        <v>603</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>77</v>
@@ -2730,8 +2818,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>576</v>
+      <c r="A33" s="7" t="s">
+        <v>603</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>80</v>
@@ -2744,11 +2832,11 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>576</v>
+      <c r="A34" s="7" t="s">
+        <v>603</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>83</v>
@@ -2758,11 +2846,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>577</v>
+      <c r="A35" s="7" t="s">
+        <v>604</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>85</v>
@@ -2772,11 +2860,11 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>577</v>
+      <c r="A36" s="7" t="s">
+        <v>604</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>87</v>
@@ -2786,8 +2874,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>577</v>
+      <c r="A37" s="7" t="s">
+        <v>604</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>89</v>
@@ -2800,8 +2888,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>578</v>
+      <c r="A38" s="7" t="s">
+        <v>605</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>92</v>
@@ -2814,11 +2902,11 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>578</v>
+      <c r="A39" s="7" t="s">
+        <v>605</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>94</v>
@@ -2828,8 +2916,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
-        <v>43720</v>
+      <c r="A40" s="7" t="s">
+        <v>577</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>96</v>
@@ -2842,11 +2930,11 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="39" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
-        <v>43720</v>
+      <c r="A41" s="7" t="s">
+        <v>577</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>99</v>
@@ -2856,8 +2944,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
-        <v>43720</v>
+      <c r="A42" s="7" t="s">
+        <v>577</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>101</v>
@@ -2870,11 +2958,11 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
-        <v>43750</v>
+      <c r="A43" s="7" t="s">
+        <v>578</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>103</v>
@@ -2884,11 +2972,11 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="39" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
-        <v>43750</v>
+      <c r="A44" s="7" t="s">
+        <v>578</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>105</v>
@@ -2898,11 +2986,11 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="12">
-        <v>43750</v>
+      <c r="A45" s="7" t="s">
+        <v>578</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>107</v>
@@ -2911,12 +2999,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13">
-        <v>43781</v>
+    <row r="46" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>579</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>109</v>
@@ -2926,8 +3014,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>579</v>
+      <c r="A47" s="7" t="s">
+        <v>606</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>111</v>
@@ -2940,8 +3028,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>579</v>
+      <c r="A48" s="7" t="s">
+        <v>606</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>113</v>
@@ -2954,8 +3042,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>579</v>
+      <c r="A49" s="7" t="s">
+        <v>606</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>116</v>
@@ -2968,11 +3056,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>580</v>
+      <c r="A50" s="8" t="s">
+        <v>607</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>118</v>
@@ -2982,11 +3070,11 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12">
-        <v>44138</v>
+      <c r="A51" s="7" t="s">
+        <v>580</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>120</v>
@@ -2996,11 +3084,11 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="12">
-        <v>44138</v>
+      <c r="A52" s="7" t="s">
+        <v>580</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>83</v>
@@ -3010,11 +3098,11 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="12">
-        <v>44138</v>
+      <c r="A53" s="7" t="s">
+        <v>580</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>123</v>
@@ -3024,11 +3112,11 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>539</v>
+      <c r="A54" s="7" t="s">
+        <v>608</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>37</v>
@@ -3038,11 +3126,11 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>539</v>
+      <c r="A55" s="7" t="s">
+        <v>608</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>126</v>
@@ -3052,11 +3140,11 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>539</v>
+      <c r="A56" s="7" t="s">
+        <v>608</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>128</v>
@@ -3066,8 +3154,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>540</v>
+      <c r="A57" s="7" t="s">
+        <v>609</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>471</v>
@@ -3080,8 +3168,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>540</v>
+      <c r="A58" s="7" t="s">
+        <v>609</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>252</v>
@@ -3094,8 +3182,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>540</v>
+      <c r="A59" s="7" t="s">
+        <v>609</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>454</v>
@@ -3108,11 +3196,11 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>541</v>
+      <c r="A60" s="7" t="s">
+        <v>610</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>134</v>
@@ -3122,11 +3210,11 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="39" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>541</v>
+      <c r="A61" s="7" t="s">
+        <v>610</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>69</v>
@@ -3136,11 +3224,11 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>541</v>
+      <c r="A62" s="7" t="s">
+        <v>610</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>137</v>
@@ -3150,11 +3238,11 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>542</v>
+      <c r="A63" s="8" t="s">
+        <v>611</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>139</v>
@@ -3164,8 +3252,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>575</v>
+      <c r="A64" s="7" t="s">
+        <v>602</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>141</v>
@@ -3178,8 +3266,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
-        <v>575</v>
+      <c r="A65" s="7" t="s">
+        <v>602</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>515</v>
@@ -3192,8 +3280,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>581</v>
+      <c r="A66" s="7" t="s">
+        <v>612</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>144</v>
@@ -3206,8 +3294,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>581</v>
+      <c r="A67" s="7" t="s">
+        <v>612</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>501</v>
@@ -3220,8 +3308,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>582</v>
+      <c r="A68" s="7" t="s">
+        <v>613</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>148</v>
@@ -3234,8 +3322,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>582</v>
+      <c r="A69" s="7" t="s">
+        <v>613</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>151</v>
@@ -3248,8 +3336,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>583</v>
+      <c r="A70" s="7" t="s">
+        <v>614</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>154</v>
@@ -3262,8 +3350,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
-        <v>583</v>
+      <c r="A71" s="7" t="s">
+        <v>614</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>514</v>
@@ -3276,8 +3364,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>584</v>
+      <c r="A72" s="7" t="s">
+        <v>615</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>502</v>
@@ -3290,8 +3378,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
-        <v>584</v>
+      <c r="A73" s="7" t="s">
+        <v>615</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>159</v>
@@ -3304,8 +3392,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>584</v>
+      <c r="A74" s="7" t="s">
+        <v>615</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>528</v>
@@ -3318,8 +3406,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>585</v>
+      <c r="A75" s="7" t="s">
+        <v>616</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>503</v>
@@ -3332,8 +3420,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>585</v>
+      <c r="A76" s="7" t="s">
+        <v>616</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>516</v>
@@ -3346,8 +3434,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>586</v>
+      <c r="A77" s="7" t="s">
+        <v>617</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>504</v>
@@ -3360,10 +3448,10 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>586</v>
-      </c>
-      <c r="B78" s="3" t="s">
+      <c r="A78" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -3374,10 +3462,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>586</v>
-      </c>
-      <c r="B79" s="3" t="s">
+      <c r="A79" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -3388,8 +3476,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="12">
-        <v>43475</v>
+      <c r="A80" s="7" t="s">
+        <v>581</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>505</v>
@@ -3402,8 +3490,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="12">
-        <v>43475</v>
+      <c r="A81" s="7" t="s">
+        <v>581</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>517</v>
@@ -3416,8 +3504,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>587</v>
+      <c r="A82" s="7" t="s">
+        <v>618</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>172</v>
@@ -3430,10 +3518,10 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
-        <v>587</v>
-      </c>
-      <c r="B83" s="3" t="s">
+      <c r="A83" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -3444,8 +3532,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>588</v>
+      <c r="A84" s="7" t="s">
+        <v>619</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>176</v>
@@ -3458,8 +3546,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
-        <v>588</v>
+      <c r="A85" s="7" t="s">
+        <v>619</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>179</v>
@@ -3472,8 +3560,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="12">
-        <v>43566</v>
+      <c r="A86" s="7" t="s">
+        <v>582</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>182</v>
@@ -3486,10 +3574,10 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="12">
-        <v>43566</v>
-      </c>
-      <c r="B87" s="3" t="s">
+      <c r="A87" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>518</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -3500,8 +3588,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="12">
-        <v>43566</v>
+      <c r="A88" s="7" t="s">
+        <v>582</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>529</v>
@@ -3514,8 +3602,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="12">
-        <v>43596</v>
+      <c r="A89" s="7" t="s">
+        <v>583</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>506</v>
@@ -3528,8 +3616,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="12">
-        <v>43596</v>
+      <c r="A90" s="7" t="s">
+        <v>583</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>519</v>
@@ -3542,8 +3630,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="12">
-        <v>43596</v>
+      <c r="A91" s="7" t="s">
+        <v>583</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>530</v>
@@ -3556,8 +3644,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="12" t="s">
-        <v>589</v>
+      <c r="A92" s="7" t="s">
+        <v>620</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>195</v>
@@ -3570,8 +3658,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="12" t="s">
-        <v>589</v>
+      <c r="A93" s="7" t="s">
+        <v>620</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>197</v>
@@ -3584,8 +3672,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
-        <v>589</v>
+      <c r="A94" s="7" t="s">
+        <v>620</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>199</v>
@@ -3598,8 +3686,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="12">
-        <v>44077</v>
+      <c r="A95" s="7" t="s">
+        <v>584</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>507</v>
@@ -3612,8 +3700,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="12">
-        <v>44077</v>
+      <c r="A96" s="7" t="s">
+        <v>584</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>520</v>
@@ -3626,8 +3714,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="12">
-        <v>44077</v>
+      <c r="A97" s="7" t="s">
+        <v>584</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>531</v>
@@ -3640,8 +3728,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="12">
-        <v>44107</v>
+      <c r="A98" s="7" t="s">
+        <v>585</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>508</v>
@@ -3654,8 +3742,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="12">
-        <v>44107</v>
+      <c r="A99" s="7" t="s">
+        <v>585</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>521</v>
@@ -3668,8 +3756,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="12">
-        <v>44107</v>
+      <c r="A100" s="7" t="s">
+        <v>585</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>532</v>
@@ -3682,8 +3770,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="12" t="s">
-        <v>590</v>
+      <c r="A101" s="7" t="s">
+        <v>621</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>508</v>
@@ -3696,8 +3784,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
-        <v>590</v>
+      <c r="A102" s="7" t="s">
+        <v>621</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>522</v>
@@ -3710,8 +3798,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>590</v>
+      <c r="A103" s="7" t="s">
+        <v>621</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>533</v>
@@ -3724,8 +3812,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
-        <v>591</v>
+      <c r="A104" s="7" t="s">
+        <v>622</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>509</v>
@@ -3738,8 +3826,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>591</v>
+      <c r="A105" s="7" t="s">
+        <v>622</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>523</v>
@@ -3752,8 +3840,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
-        <v>591</v>
+      <c r="A106" s="7" t="s">
+        <v>622</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>534</v>
@@ -3766,8 +3854,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>592</v>
+      <c r="A107" s="7" t="s">
+        <v>623</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>510</v>
@@ -3775,13 +3863,13 @@
       <c r="C107" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
-        <v>592</v>
+      <c r="A108" s="7" t="s">
+        <v>623</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>524</v>
@@ -3789,13 +3877,13 @@
       <c r="C108" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="D108" s="3" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="12" t="s">
-        <v>592</v>
+      <c r="A109" s="7" t="s">
+        <v>623</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>535</v>
@@ -3803,13 +3891,13 @@
       <c r="C109" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="3" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
-        <v>593</v>
+      <c r="A110" s="7" t="s">
+        <v>624</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>457</v>
@@ -3817,13 +3905,13 @@
       <c r="C110" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="3" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="12" t="s">
-        <v>593</v>
+      <c r="A111" s="7" t="s">
+        <v>624</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>525</v>
@@ -3831,13 +3919,13 @@
       <c r="C111" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="3" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
-        <v>593</v>
+      <c r="A112" s="7" t="s">
+        <v>624</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>536</v>
@@ -3845,13 +3933,13 @@
       <c r="C112" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="12" t="s">
-        <v>594</v>
+      <c r="A113" s="7" t="s">
+        <v>625</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>511</v>
@@ -3859,13 +3947,13 @@
       <c r="C113" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D113" s="3" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
-        <v>594</v>
+      <c r="A114" s="7" t="s">
+        <v>625</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>526</v>
@@ -3873,13 +3961,13 @@
       <c r="C114" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="12" t="s">
-        <v>594</v>
+      <c r="A115" s="7" t="s">
+        <v>625</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>537</v>
@@ -3887,13 +3975,13 @@
       <c r="C115" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D115" s="4" t="s">
+      <c r="D115" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="12" t="s">
-        <v>594</v>
+      <c r="A116" s="7" t="s">
+        <v>625</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>227</v>
@@ -3901,13 +3989,13 @@
       <c r="C116" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="12" t="s">
-        <v>595</v>
+      <c r="A117" s="7" t="s">
+        <v>626</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>512</v>
@@ -3915,13 +4003,13 @@
       <c r="C117" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="12" t="s">
-        <v>595</v>
+      <c r="A118" s="7" t="s">
+        <v>626</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>527</v>
@@ -3929,13 +4017,13 @@
       <c r="C118" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="12" t="s">
-        <v>595</v>
+      <c r="A119" s="7" t="s">
+        <v>626</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>538</v>
@@ -3943,13 +4031,13 @@
       <c r="C119" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="12" t="s">
-        <v>596</v>
+      <c r="A120" s="7" t="s">
+        <v>627</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>513</v>
@@ -3957,13 +4045,13 @@
       <c r="C120" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="12">
-        <v>43686</v>
+      <c r="A121" s="7" t="s">
+        <v>586</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>235</v>
@@ -3976,8 +4064,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="12">
-        <v>43686</v>
+      <c r="A122" s="7" t="s">
+        <v>586</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>237</v>
@@ -3990,8 +4078,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="12">
-        <v>43717</v>
+      <c r="A123" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>239</v>
@@ -4004,8 +4092,8 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="12">
-        <v>43717</v>
+      <c r="A124" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>470</v>
@@ -4018,8 +4106,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="12">
-        <v>43747</v>
+      <c r="A125" s="7" t="s">
+        <v>574</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>452</v>
@@ -4032,8 +4120,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="12">
-        <v>43747</v>
+      <c r="A126" s="7" t="s">
+        <v>574</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>246</v>
@@ -4046,8 +4134,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="12">
-        <v>43778</v>
+      <c r="A127" s="7" t="s">
+        <v>575</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>248</v>
@@ -4060,8 +4148,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="12">
-        <v>43778</v>
+      <c r="A128" s="7" t="s">
+        <v>575</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>250</v>
@@ -4074,8 +4162,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="12">
-        <v>43808</v>
+      <c r="A129" s="7" t="s">
+        <v>576</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>252</v>
@@ -4088,8 +4176,8 @@
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="12">
-        <v>43808</v>
+      <c r="A130" s="7" t="s">
+        <v>576</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>254</v>
@@ -4102,8 +4190,8 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
-        <v>597</v>
+      <c r="A131" s="7" t="s">
+        <v>628</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>257</v>
@@ -4116,8 +4204,8 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="12" t="s">
-        <v>597</v>
+      <c r="A132" s="7" t="s">
+        <v>628</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>259</v>
@@ -4130,8 +4218,8 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="12" t="s">
-        <v>597</v>
+      <c r="A133" s="7" t="s">
+        <v>628</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>262</v>
@@ -4144,8 +4232,8 @@
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="12" t="s">
-        <v>574</v>
+      <c r="A134" s="7" t="s">
+        <v>601</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>453</v>
@@ -4158,8 +4246,8 @@
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="12" t="s">
-        <v>574</v>
+      <c r="A135" s="7" t="s">
+        <v>601</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>471</v>
@@ -4172,8 +4260,8 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="12" t="s">
-        <v>574</v>
+      <c r="A136" s="7" t="s">
+        <v>601</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>488</v>
@@ -4186,8 +4274,8 @@
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="12" t="s">
-        <v>575</v>
+      <c r="A137" s="7" t="s">
+        <v>602</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>454</v>
@@ -4200,8 +4288,8 @@
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="12" t="s">
-        <v>575</v>
+      <c r="A138" s="7" t="s">
+        <v>602</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>472</v>
@@ -4214,8 +4302,8 @@
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="12" t="s">
-        <v>575</v>
+      <c r="A139" s="7" t="s">
+        <v>602</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>464</v>
@@ -4228,8 +4316,8 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="12" t="s">
-        <v>581</v>
+      <c r="A140" s="7" t="s">
+        <v>612</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>468</v>
@@ -4242,8 +4330,8 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="12" t="s">
-        <v>581</v>
+      <c r="A141" s="7" t="s">
+        <v>612</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>473</v>
@@ -4256,8 +4344,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="13" t="s">
-        <v>582</v>
+      <c r="A142" s="8" t="s">
+        <v>613</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>277</v>
@@ -4269,9 +4357,9 @@
         <v>278</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="15">
-        <v>43687</v>
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="9" t="s">
+        <v>587</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>455</v>
@@ -4283,8 +4371,10 @@
         <v>280</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="16"/>
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="9" t="s">
+        <v>587</v>
+      </c>
       <c r="B144" s="1" t="s">
         <v>474</v>
       </c>
@@ -4295,8 +4385,10 @@
         <v>281</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="17"/>
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="9" t="s">
+        <v>587</v>
+      </c>
       <c r="B145" s="1" t="s">
         <v>489</v>
       </c>
@@ -4307,9 +4399,9 @@
         <v>282</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="15">
-        <v>43718</v>
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="9" t="s">
+        <v>588</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>283</v>
@@ -4321,8 +4413,10 @@
         <v>284</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="16"/>
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="9" t="s">
+        <v>588</v>
+      </c>
       <c r="B147" s="1" t="s">
         <v>475</v>
       </c>
@@ -4333,8 +4427,10 @@
         <v>285</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="17"/>
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="9" t="s">
+        <v>588</v>
+      </c>
       <c r="B148" s="1" t="s">
         <v>490</v>
       </c>
@@ -4345,9 +4441,9 @@
         <v>286</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="15">
-        <v>43748</v>
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="9" t="s">
+        <v>589</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>456</v>
@@ -4359,8 +4455,10 @@
         <v>288</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="16"/>
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="9" t="s">
+        <v>589</v>
+      </c>
       <c r="B150" s="1" t="s">
         <v>289</v>
       </c>
@@ -4371,8 +4469,10 @@
         <v>290</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="17"/>
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="9" t="s">
+        <v>589</v>
+      </c>
       <c r="B151" s="1" t="s">
         <v>491</v>
       </c>
@@ -4383,9 +4483,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="15">
-        <v>43750</v>
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>578</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>469</v>
@@ -4397,8 +4497,10 @@
         <v>292</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="16"/>
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="9" t="s">
+        <v>578</v>
+      </c>
       <c r="B153" s="1" t="s">
         <v>476</v>
       </c>
@@ -4409,8 +4511,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="17"/>
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="9" t="s">
+        <v>578</v>
+      </c>
       <c r="B154" s="1" t="s">
         <v>492</v>
       </c>
@@ -4422,8 +4526,8 @@
       </c>
     </row>
     <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="13">
-        <v>43781</v>
+      <c r="A155" s="8" t="s">
+        <v>579</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>296</v>
@@ -4435,9 +4539,9 @@
         <v>297</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="15" t="s">
-        <v>598</v>
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="9" t="s">
+        <v>629</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>298</v>
@@ -4449,8 +4553,10 @@
         <v>299</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="17"/>
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="9" t="s">
+        <v>629</v>
+      </c>
       <c r="B157" s="1" t="s">
         <v>300</v>
       </c>
@@ -4461,9 +4567,9 @@
         <v>301</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="15" t="s">
-        <v>599</v>
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="9" t="s">
+        <v>630</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>457</v>
@@ -4475,8 +4581,10 @@
         <v>302</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="16"/>
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="9" t="s">
+        <v>630</v>
+      </c>
       <c r="B159" s="1" t="s">
         <v>477</v>
       </c>
@@ -4487,8 +4595,10 @@
         <v>303</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="17"/>
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="9" t="s">
+        <v>630</v>
+      </c>
       <c r="B160" s="1" t="s">
         <v>493</v>
       </c>
@@ -4499,9 +4609,9 @@
         <v>304</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="15" t="s">
-        <v>600</v>
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="9" t="s">
+        <v>631</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>458</v>
@@ -4513,8 +4623,10 @@
         <v>305</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="16"/>
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="9" t="s">
+        <v>631</v>
+      </c>
       <c r="B162" s="1" t="s">
         <v>478</v>
       </c>
@@ -4525,8 +4637,10 @@
         <v>306</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="17"/>
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="9" t="s">
+        <v>631</v>
+      </c>
       <c r="B163" s="1" t="s">
         <v>494</v>
       </c>
@@ -4537,9 +4651,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="15">
-        <v>44082</v>
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="9" t="s">
+        <v>590</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>459</v>
@@ -4551,8 +4665,10 @@
         <v>309</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="16"/>
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="9" t="s">
+        <v>590</v>
+      </c>
       <c r="B165" s="1" t="s">
         <v>479</v>
       </c>
@@ -4563,8 +4679,10 @@
         <v>310</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="17"/>
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="9" t="s">
+        <v>590</v>
+      </c>
       <c r="B166" s="1" t="s">
         <v>495</v>
       </c>
@@ -4575,9 +4693,9 @@
         <v>311</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="15">
-        <v>44112</v>
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="9" t="s">
+        <v>591</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>460</v>
@@ -4589,8 +4707,10 @@
         <v>312</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="17"/>
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="9" t="s">
+        <v>591</v>
+      </c>
       <c r="B168" s="1" t="s">
         <v>480</v>
       </c>
@@ -4601,9 +4721,9 @@
         <v>313</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="15" t="s">
-        <v>601</v>
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="9" t="s">
+        <v>632</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>461</v>
@@ -4615,8 +4735,10 @@
         <v>314</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="16"/>
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="9" t="s">
+        <v>632</v>
+      </c>
       <c r="B170" s="1" t="s">
         <v>481</v>
       </c>
@@ -4627,8 +4749,10 @@
         <v>315</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="17"/>
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="9" t="s">
+        <v>632</v>
+      </c>
       <c r="B171" s="1" t="s">
         <v>496</v>
       </c>
@@ -4639,73 +4763,79 @@
         <v>317</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="15" t="s">
-        <v>602</v>
-      </c>
-      <c r="B172" s="5" t="s">
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="B172" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="C172" s="5" t="s">
+      <c r="C172" s="4" t="s">
         <v>319</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="16"/>
-      <c r="B173" s="5" t="s">
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="B173" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="C173" s="5" t="s">
+      <c r="C173" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="17"/>
-      <c r="B174" s="5" t="s">
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="B174" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C174" s="5" t="s">
+      <c r="C174" s="4" t="s">
         <v>324</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="15" t="s">
-        <v>603</v>
-      </c>
-      <c r="B175" s="5" t="s">
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="B175" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="C175" s="5" t="s">
+      <c r="C175" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="17"/>
-      <c r="B176" s="5" t="s">
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="B176" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="C176" s="5" t="s">
+      <c r="C176" s="4" t="s">
         <v>329</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="15">
-        <v>44531</v>
+    <row r="177" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="9" t="s">
+        <v>592</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>318</v>
@@ -4713,37 +4843,41 @@
       <c r="C177" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D177" s="4" t="s">
+      <c r="D177" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="16"/>
+    <row r="178" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="9" t="s">
+        <v>592</v>
+      </c>
       <c r="B178" s="1" t="s">
         <v>321</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D178" s="4" t="s">
+      <c r="D178" s="3" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="17"/>
+    <row r="179" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="9" t="s">
+        <v>592</v>
+      </c>
       <c r="B179" s="1" t="s">
         <v>323</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D179" s="4" t="s">
+      <c r="D179" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="15" t="s">
-        <v>604</v>
+    <row r="180" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="9" t="s">
+        <v>635</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>462</v>
@@ -4751,37 +4885,41 @@
       <c r="C180" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D180" s="4" t="s">
+      <c r="D180" s="3" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="16"/>
+    <row r="181" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="9" t="s">
+        <v>635</v>
+      </c>
       <c r="B181" s="1" t="s">
         <v>482</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D181" s="4" t="s">
+      <c r="D181" s="3" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="17"/>
+    <row r="182" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="9" t="s">
+        <v>635</v>
+      </c>
       <c r="B182" s="1" t="s">
         <v>497</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D182" s="4" t="s">
+      <c r="D182" s="3" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="15" t="s">
-        <v>593</v>
+    <row r="183" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="9" t="s">
+        <v>624</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>463</v>
@@ -4789,25 +4927,27 @@
       <c r="C183" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D183" s="4" t="s">
+      <c r="D183" s="3" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="17"/>
+    <row r="184" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="9" t="s">
+        <v>624</v>
+      </c>
       <c r="B184" s="1" t="s">
         <v>483</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D184" s="4" t="s">
+      <c r="D184" s="3" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="15" t="s">
-        <v>594</v>
+    <row r="185" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="9" t="s">
+        <v>625</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>464</v>
@@ -4815,25 +4955,27 @@
       <c r="C185" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D185" s="4" t="s">
+      <c r="D185" s="3" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="17"/>
+    <row r="186" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="9" t="s">
+        <v>625</v>
+      </c>
       <c r="B186" s="1" t="s">
         <v>484</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D186" s="4" t="s">
+      <c r="D186" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="15" t="s">
-        <v>605</v>
+    <row r="187" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="9" t="s">
+        <v>636</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>465</v>
@@ -4841,37 +4983,41 @@
       <c r="C187" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D187" s="4" t="s">
+      <c r="D187" s="3" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="16"/>
+    <row r="188" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="9" t="s">
+        <v>636</v>
+      </c>
       <c r="B188" s="1" t="s">
         <v>485</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D188" s="4" t="s">
+      <c r="D188" s="3" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="17"/>
+    <row r="189" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="9" t="s">
+        <v>636</v>
+      </c>
       <c r="B189" s="1" t="s">
         <v>498</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D189" s="4" t="s">
+      <c r="D189" s="3" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="15">
-        <v>44411</v>
+    <row r="190" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="9" t="s">
+        <v>593</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>466</v>
@@ -4879,37 +5025,41 @@
       <c r="C190" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D190" s="4" t="s">
+      <c r="D190" s="3" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="16"/>
+    <row r="191" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="9" t="s">
+        <v>593</v>
+      </c>
       <c r="B191" s="1" t="s">
         <v>486</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D191" s="4" t="s">
+      <c r="D191" s="3" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="17"/>
+    <row r="192" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="9" t="s">
+        <v>593</v>
+      </c>
       <c r="B192" s="1" t="s">
         <v>499</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D192" s="4" t="s">
+      <c r="D192" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="15">
-        <v>44442</v>
+    <row r="193" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="9" t="s">
+        <v>594</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>467</v>
@@ -4917,37 +5067,41 @@
       <c r="C193" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D193" s="4" t="s">
+      <c r="D193" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="16"/>
+    <row r="194" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="9" t="s">
+        <v>594</v>
+      </c>
       <c r="B194" s="1" t="s">
         <v>487</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D194" s="4" t="s">
+      <c r="D194" s="3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="17"/>
+    <row r="195" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="9" t="s">
+        <v>594</v>
+      </c>
       <c r="B195" s="1" t="s">
         <v>500</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D195" s="4" t="s">
+      <c r="D195" s="3" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="8" t="s">
-        <v>584</v>
+      <c r="A196" s="9" t="s">
+        <v>615</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>353</v>
@@ -4960,8 +5114,8 @@
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="8" t="s">
-        <v>584</v>
+      <c r="A197" s="9" t="s">
+        <v>615</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>353</v>
@@ -4974,8 +5128,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="6" t="s">
-        <v>585</v>
+      <c r="A198" s="9" t="s">
+        <v>616</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>429</v>
@@ -4988,8 +5142,8 @@
       </c>
     </row>
     <row r="199" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="6" t="s">
-        <v>585</v>
+      <c r="A199" s="9" t="s">
+        <v>616</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>358</v>
@@ -5002,8 +5156,8 @@
       </c>
     </row>
     <row r="200" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="6" t="s">
-        <v>606</v>
+      <c r="A200" s="9" t="s">
+        <v>637</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>360</v>
@@ -5016,8 +5170,8 @@
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="6" t="s">
-        <v>606</v>
+      <c r="A201" s="9" t="s">
+        <v>637</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>363</v>
@@ -5030,8 +5184,8 @@
       </c>
     </row>
     <row r="202" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="6" t="s">
-        <v>607</v>
+      <c r="A202" s="9" t="s">
+        <v>638</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>366</v>
@@ -5044,8 +5198,8 @@
       </c>
     </row>
     <row r="203" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="6" t="s">
-        <v>607</v>
+      <c r="A203" s="9" t="s">
+        <v>638</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>368</v>
@@ -5058,8 +5212,8 @@
       </c>
     </row>
     <row r="204" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="6" t="s">
-        <v>586</v>
+      <c r="A204" s="9" t="s">
+        <v>617</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>430</v>
@@ -5072,8 +5226,8 @@
       </c>
     </row>
     <row r="205" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="6" t="s">
-        <v>586</v>
+      <c r="A205" s="9" t="s">
+        <v>617</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>371</v>
@@ -5086,8 +5240,8 @@
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="6" t="s">
-        <v>586</v>
+      <c r="A206" s="9" t="s">
+        <v>617</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>373</v>
@@ -5100,8 +5254,8 @@
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="9">
-        <v>43475</v>
+      <c r="A207" s="9" t="s">
+        <v>581</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>376</v>
@@ -5114,8 +5268,8 @@
       </c>
     </row>
     <row r="208" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="9">
-        <v>43475</v>
+      <c r="A208" s="13" t="s">
+        <v>581</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>379</v>
@@ -5128,22 +5282,22 @@
       </c>
     </row>
     <row r="209" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="9">
-        <v>43475</v>
-      </c>
-      <c r="B209" s="1" t="s">
+      <c r="A209" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="B209" s="14" t="s">
         <v>431</v>
       </c>
-      <c r="C209" s="1" t="s">
-        <v>49</v>
+      <c r="C209" s="14" t="s">
+        <v>643</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="9">
-        <v>43506</v>
+      <c r="A210" s="9" t="s">
+        <v>595</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>382</v>
@@ -5156,8 +5310,8 @@
       </c>
     </row>
     <row r="211" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="9">
-        <v>43506</v>
+      <c r="A211" s="9" t="s">
+        <v>595</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>385</v>
@@ -5170,8 +5324,8 @@
       </c>
     </row>
     <row r="212" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="9">
-        <v>43506</v>
+      <c r="A212" s="9" t="s">
+        <v>595</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>387</v>
@@ -5184,8 +5338,8 @@
       </c>
     </row>
     <row r="213" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="9">
-        <v>43534</v>
+      <c r="A213" s="9" t="s">
+        <v>596</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>389</v>
@@ -5198,8 +5352,8 @@
       </c>
     </row>
     <row r="214" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="9">
-        <v>43534</v>
+      <c r="A214" s="9" t="s">
+        <v>596</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>433</v>
@@ -5212,8 +5366,8 @@
       </c>
     </row>
     <row r="215" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="9">
-        <v>43534</v>
+      <c r="A215" s="9" t="s">
+        <v>596</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>434</v>
@@ -5225,9 +5379,9 @@
         <v>392</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="9">
-        <v>43627</v>
+    <row r="216" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="9" t="s">
+        <v>597</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>393</v>
@@ -5240,8 +5394,8 @@
       </c>
     </row>
     <row r="217" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="9">
-        <v>43627</v>
+      <c r="A217" s="9" t="s">
+        <v>597</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>432</v>
@@ -5254,8 +5408,8 @@
       </c>
     </row>
     <row r="218" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="9">
-        <v>43657</v>
+      <c r="A218" s="9" t="s">
+        <v>598</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>396</v>
@@ -5268,8 +5422,8 @@
       </c>
     </row>
     <row r="219" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="9">
-        <v>43657</v>
+      <c r="A219" s="9" t="s">
+        <v>598</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>398</v>
@@ -5282,8 +5436,8 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="6" t="s">
-        <v>589</v>
+      <c r="A220" s="9" t="s">
+        <v>620</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>400</v>
@@ -5296,8 +5450,8 @@
       </c>
     </row>
     <row r="221" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="6" t="s">
-        <v>589</v>
+      <c r="A221" s="9" t="s">
+        <v>620</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>402</v>
@@ -5310,8 +5464,8 @@
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="2" t="s">
-        <v>579</v>
+      <c r="A222" s="10" t="s">
+        <v>606</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>404</v>
@@ -5324,8 +5478,8 @@
       </c>
     </row>
     <row r="223" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="6" t="s">
-        <v>608</v>
+      <c r="A223" s="9" t="s">
+        <v>639</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>439</v>
@@ -5338,8 +5492,8 @@
       </c>
     </row>
     <row r="224" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="6" t="s">
-        <v>608</v>
+      <c r="A224" s="9" t="s">
+        <v>639</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>435</v>
@@ -5352,8 +5506,8 @@
       </c>
     </row>
     <row r="225" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="6" t="s">
-        <v>608</v>
+      <c r="A225" s="9" t="s">
+        <v>639</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>447</v>
@@ -5366,8 +5520,8 @@
       </c>
     </row>
     <row r="226" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="10">
-        <v>44021</v>
+      <c r="A226" s="10" t="s">
+        <v>599</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>440</v>
@@ -5380,10 +5534,10 @@
       </c>
     </row>
     <row r="227" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="10">
-        <v>44021</v>
-      </c>
-      <c r="B227" s="3" t="s">
+      <c r="A227" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="B227" s="2" t="s">
         <v>442</v>
       </c>
       <c r="C227" s="1" t="s">
@@ -5394,8 +5548,8 @@
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="10">
-        <v>44021</v>
+      <c r="A228" s="10" t="s">
+        <v>599</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>448</v>
@@ -5408,8 +5562,8 @@
       </c>
     </row>
     <row r="229" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="6" t="s">
-        <v>609</v>
+      <c r="A229" s="9" t="s">
+        <v>640</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>436</v>
@@ -5422,10 +5576,10 @@
       </c>
     </row>
     <row r="230" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="B230" s="3" t="s">
+      <c r="A230" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>443</v>
       </c>
       <c r="C230" s="1" t="s">
@@ -5436,10 +5590,10 @@
       </c>
     </row>
     <row r="231" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="B231" s="3" t="s">
+      <c r="A231" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="B231" s="2" t="s">
         <v>449</v>
       </c>
       <c r="C231" s="1" t="s">
@@ -5450,10 +5604,10 @@
       </c>
     </row>
     <row r="232" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="6" t="s">
-        <v>610</v>
-      </c>
-      <c r="B232" s="3" t="s">
+      <c r="A232" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="B232" s="2" t="s">
         <v>441</v>
       </c>
       <c r="C232" s="1" t="s">
@@ -5464,10 +5618,10 @@
       </c>
     </row>
     <row r="233" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="6" t="s">
-        <v>610</v>
-      </c>
-      <c r="B233" s="3" t="s">
+      <c r="A233" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="B233" s="2" t="s">
         <v>444</v>
       </c>
       <c r="C233" s="1" t="s">
@@ -5478,10 +5632,10 @@
       </c>
     </row>
     <row r="234" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="6" t="s">
-        <v>610</v>
-      </c>
-      <c r="B234" s="3" t="s">
+      <c r="A234" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="B234" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C234" s="1" t="s">
@@ -5492,8 +5646,8 @@
       </c>
     </row>
     <row r="235" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="6" t="s">
-        <v>596</v>
+      <c r="A235" s="9" t="s">
+        <v>627</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>437</v>
@@ -5506,8 +5660,8 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="6" t="s">
-        <v>596</v>
+      <c r="A236" s="9" t="s">
+        <v>627</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>445</v>
@@ -5520,8 +5674,8 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="6" t="s">
-        <v>596</v>
+      <c r="A237" s="9" t="s">
+        <v>627</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>451</v>
@@ -5534,8 +5688,8 @@
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="6" t="s">
-        <v>611</v>
+      <c r="A238" s="9" t="s">
+        <v>642</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>438</v>
@@ -5548,8 +5702,8 @@
       </c>
     </row>
     <row r="239" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="6" t="s">
-        <v>611</v>
+      <c r="A239" s="9" t="s">
+        <v>642</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>446</v>
@@ -5562,27 +5716,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A193:A195"/>
-    <mergeCell ref="A177:A179"/>
-    <mergeCell ref="A180:A182"/>
-    <mergeCell ref="A183:A184"/>
-    <mergeCell ref="A185:A186"/>
-    <mergeCell ref="A187:A189"/>
-    <mergeCell ref="A190:A192"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="A164:A166"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="A169:A171"/>
-    <mergeCell ref="A172:A174"/>
-    <mergeCell ref="A175:A176"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A148"/>
-    <mergeCell ref="A149:A151"/>
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="A156:A157"/>
-    <mergeCell ref="A158:A160"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>